<commit_message>
modified:   WebRoot/js/common.js 	modified:   WebRoot/page/bid/addbid.jsp 	modified:   WebRoot/page/bid/updbid.jsp 	modified:   WebRoot/page/bidaudit.xlsx 	modified:   WebRoot/page/bidregister.xlsx 	modified:   src/com/cn/common/factory/PoiBidAudit.java 	modified:   src/com/cn/common/factory/PoiBidRegister.java 	modified:   src/com/cn/tbps/dto/BidCompDto.java 	modified:   src/config/ibatis/tbps-bidcomp.xml
</commit_message>
<xml_diff>
--- a/WebRoot/page/bidaudit.xlsx
+++ b/WebRoot/page/bidaudit.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Homework\sh_prj\tbps\WebRoot\page\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18240" windowHeight="4395"/>
   </bookViews>
@@ -93,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -466,7 +461,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -564,15 +559,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -593,10 +579,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="常规 3" xfId="3"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -658,7 +644,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -700,7 +686,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -735,7 +721,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -947,10 +933,10 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="50.1" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="2.75" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.25" style="3" customWidth="1"/>
@@ -958,30 +944,30 @@
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="22" customFormat="1" ht="39" customHeight="1">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" s="22" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-    </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" ht="31.5" customHeight="1" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" s="22" customFormat="1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-    </row>
-    <row r="3" spans="1:7" s="22" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A3" s="39" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" spans="1:7" s="22" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="36" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -1003,8 +989,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1">
-      <c r="A4" s="40"/>
+    <row r="4" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="37"/>
       <c r="B4" s="21" t="s">
         <v>8</v>
       </c>
@@ -1014,7 +1000,7 @@
       <c r="F4" s="27"/>
       <c r="G4" s="28"/>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="29">
         <v>1</v>
       </c>
@@ -1025,7 +1011,7 @@
       <c r="F5" s="27"/>
       <c r="G5" s="28"/>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="6" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="29">
         <v>2</v>
       </c>
@@ -1036,7 +1022,7 @@
       <c r="F6" s="27"/>
       <c r="G6" s="28"/>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="7" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="29">
         <v>3</v>
       </c>
@@ -1047,7 +1033,7 @@
       <c r="F7" s="27"/>
       <c r="G7" s="28"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="8" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="29">
         <v>4</v>
       </c>
@@ -1058,7 +1044,7 @@
       <c r="F8" s="27"/>
       <c r="G8" s="28"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="9" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="29">
         <v>5</v>
       </c>
@@ -1069,7 +1055,7 @@
       <c r="F9" s="27"/>
       <c r="G9" s="28"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="10" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="29">
         <v>6</v>
       </c>
@@ -1080,7 +1066,7 @@
       <c r="F10" s="27"/>
       <c r="G10" s="28"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="29">
         <v>7</v>
       </c>
@@ -1091,7 +1077,7 @@
       <c r="F11" s="19"/>
       <c r="G11" s="18"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="12" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="29">
         <v>8</v>
       </c>
@@ -1102,7 +1088,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="18"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="13" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="29">
         <v>9</v>
       </c>
@@ -1113,51 +1099,51 @@
       <c r="F13" s="13"/>
       <c r="G13" s="18"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="14" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="29">
         <v>10</v>
       </c>
       <c r="B14" s="20"/>
-      <c r="C14" s="35"/>
+      <c r="C14" s="32"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="35"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="19"/>
-      <c r="G14" s="36"/>
-    </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="30"/>
       <c r="B15" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-    </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="F15" s="19"/>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="16" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="30"/>
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="35"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="35"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="19"/>
-      <c r="G16" s="36"/>
-    </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="G16" s="33"/>
+    </row>
+    <row r="17" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="30"/>
       <c r="B17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="35"/>
+      <c r="E17" s="32"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="36"/>
-    </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+      <c r="G17" s="33"/>
+    </row>
+    <row r="18" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="14"/>
       <c r="B18" s="13" t="s">
         <v>7</v>
@@ -1168,7 +1154,7 @@
       <c r="F18" s="19"/>
       <c r="G18" s="18"/>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="19" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14"/>
       <c r="B19" s="13" t="s">
         <v>6</v>
@@ -1179,7 +1165,7 @@
       <c r="F19" s="19"/>
       <c r="G19" s="18"/>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="20" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="14"/>
       <c r="B20" s="13" t="s">
         <v>0</v>
@@ -1190,7 +1176,7 @@
       <c r="F20" s="19"/>
       <c r="G20" s="18"/>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="21" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="14"/>
       <c r="B21" s="13" t="s">
         <v>5</v>
@@ -1201,7 +1187,7 @@
       <c r="F21" s="19"/>
       <c r="G21" s="18"/>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="22" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="14"/>
       <c r="B22" s="13" t="s">
         <v>1</v>
@@ -1212,7 +1198,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1">
+    <row r="23" spans="1:7" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="14"/>
       <c r="B23" s="13" t="s">
         <v>4</v>
@@ -1223,7 +1209,7 @@
       <c r="F23" s="11"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="24" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="8" t="s">
         <v>3</v>
@@ -1244,7 +1230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="4" customFormat="1" ht="27" customHeight="1">
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>

</xml_diff>